<commit_message>
code fixes for scheduling
</commit_message>
<xml_diff>
--- a/MasterData/9. AmortTemplateTelemundo.xlsx
+++ b/MasterData/9. AmortTemplateTelemundo.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="61">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>TitleType Episode not found in drop down</t>
+  </si>
+  <si>
+    <t>Episodes need to be added but no episodes tab</t>
+  </si>
+  <si>
+    <t>Finance type doesn’t exist in dropdown</t>
   </si>
 </sst>
 </file>
@@ -2799,9 +2805,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2868,7 +2877,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42</v>
       </c>
@@ -2913,7 +2922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42</v>
       </c>
@@ -2959,7 +2968,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42</v>
       </c>
@@ -3005,7 +3014,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42</v>
       </c>
@@ -3051,7 +3060,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42</v>
       </c>
@@ -3092,9 +3101,11 @@
         <f t="shared" si="0"/>
         <v>421 RUNSportsAcquired Films</v>
       </c>
-      <c r="N6" s="1" t="e">
-        <f>VLOOKUP(M6,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3138,9 +3149,11 @@
         <f t="shared" si="0"/>
         <v>421 RUNVarietyAcquired Films</v>
       </c>
-      <c r="N7" s="1" t="e">
-        <f>VLOOKUP(M7,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3189,7 +3202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43</v>
       </c>
@@ -3281,7 +3294,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44</v>
       </c>
@@ -3327,7 +3340,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44</v>
       </c>
@@ -3419,7 +3432,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>55</v>
       </c>
@@ -3467,7 +3480,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>55</v>
       </c>
@@ -3515,7 +3528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>55</v>
       </c>
@@ -3563,7 +3576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>55</v>
       </c>
@@ -3657,7 +3670,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>190</v>
       </c>
@@ -3703,7 +3716,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>191</v>
       </c>
@@ -3751,7 +3764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>191</v>
       </c>
@@ -3797,7 +3810,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>191</v>
       </c>
@@ -3843,7 +3856,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>191</v>
       </c>
@@ -3884,12 +3897,14 @@
         <f t="shared" si="0"/>
         <v>1911 RUN-SeriesSportsAcquired Series</v>
       </c>
-      <c r="N23" s="1" t="e">
-        <f>VLOOKUP(M23,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>192</v>
       </c>
@@ -3935,7 +3950,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>193</v>
       </c>
@@ -3983,7 +3998,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>193</v>
       </c>
@@ -4029,7 +4044,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>193</v>
       </c>
@@ -4213,7 +4228,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>197</v>
       </c>
@@ -4259,7 +4274,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>198</v>
       </c>
@@ -4307,7 +4322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>198</v>
       </c>
@@ -4353,7 +4368,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>198</v>
       </c>
@@ -4445,7 +4460,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>199</v>
       </c>
@@ -4491,7 +4506,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>200</v>
       </c>
@@ -4539,7 +4554,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>200</v>
       </c>
@@ -4585,7 +4600,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>200</v>
       </c>
@@ -4769,7 +4784,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>204</v>
       </c>
@@ -4815,7 +4830,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>205</v>
       </c>
@@ -4863,7 +4878,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>205</v>
       </c>
@@ -4909,7 +4924,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>205</v>
       </c>
@@ -5001,7 +5016,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>206</v>
       </c>
@@ -5047,7 +5062,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>207</v>
       </c>
@@ -5095,7 +5110,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>207</v>
       </c>
@@ -5141,7 +5156,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>207</v>
       </c>
@@ -5279,7 +5294,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>210</v>
       </c>
@@ -5327,7 +5342,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>210</v>
       </c>
@@ -5375,7 +5390,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>211</v>
       </c>
@@ -5423,7 +5438,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>212</v>
       </c>
@@ -5471,7 +5486,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>213</v>
       </c>
@@ -5519,7 +5534,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>213</v>
       </c>
@@ -5567,7 +5582,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>213</v>
       </c>
@@ -5615,7 +5630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>213</v>
       </c>
@@ -5663,7 +5678,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>214</v>
       </c>
@@ -5711,7 +5726,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>215</v>
       </c>
@@ -5759,7 +5774,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>215</v>
       </c>
@@ -5807,7 +5822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>215</v>
       </c>
@@ -5855,7 +5870,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>215</v>
       </c>
@@ -5903,7 +5918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>216</v>
       </c>
@@ -5997,7 +6012,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>218</v>
       </c>
@@ -6089,7 +6104,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>220</v>
       </c>
@@ -6135,7 +6150,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>221</v>
       </c>
@@ -6183,7 +6198,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>221</v>
       </c>
@@ -6229,7 +6244,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>221</v>
       </c>
@@ -6321,7 +6336,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>222</v>
       </c>
@@ -6367,7 +6382,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>223</v>
       </c>
@@ -6415,7 +6430,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>223</v>
       </c>
@@ -6461,7 +6476,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>223</v>
       </c>
@@ -6599,7 +6614,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>346</v>
       </c>
@@ -6645,7 +6660,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>347</v>
       </c>
@@ -6691,7 +6706,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>348</v>
       </c>
@@ -6737,7 +6752,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>349</v>
       </c>
@@ -6785,7 +6800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>350</v>
       </c>
@@ -6833,7 +6848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>351</v>
       </c>
@@ -6874,12 +6889,11 @@
         <f t="shared" si="1"/>
         <v>3511 RUN-SpecialSpecialOriginal Specials</v>
       </c>
-      <c r="N87" s="1" t="e">
-        <f>VLOOKUP(M87,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N87" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>352</v>
       </c>
@@ -6925,7 +6939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>353</v>
       </c>
@@ -6971,7 +6985,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>354</v>
       </c>
@@ -7019,7 +7033,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>369</v>
       </c>
@@ -7066,6 +7080,21 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O91">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Film"/>
+        <filter val="News"/>
+        <filter val="Sports"/>
+        <filter val="Variety"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters>
+        <filter val="#N/A"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -7076,10 +7105,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7128,6 +7157,363 @@
         <v>421 RUNFilmAcquired Films</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>351</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F59" si="0">CONCATENATE(A3,B3,C3,D3)</f>
+        <v>3511 RUN-SpecialSpecialOriginal Specials</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code changes for white slot
</commit_message>
<xml_diff>
--- a/MasterData/9. AmortTemplateTelemundo.xlsx
+++ b/MasterData/9. AmortTemplateTelemundo.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="61">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -2808,8 +2808,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +2922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>190</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>191</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>191</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>192</v>
       </c>
@@ -4039,9 +4039,8 @@
         <f t="shared" si="0"/>
         <v>1931 RUNSeriesSports</v>
       </c>
-      <c r="N26" s="1" t="e">
-        <f>VLOOKUP(M26,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N26" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -4085,12 +4084,11 @@
         <f t="shared" si="0"/>
         <v>1931 RUNSpecialSports</v>
       </c>
-      <c r="N27" s="1" t="e">
-        <f>VLOOKUP(M27,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>193</v>
       </c>
@@ -4131,9 +4129,8 @@
         <f t="shared" si="0"/>
         <v>1931 RUNSportsSports</v>
       </c>
-      <c r="N28" s="1" t="e">
-        <f>VLOOKUP(M28,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N28" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -4228,7 +4225,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>197</v>
       </c>
@@ -4322,7 +4319,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>198</v>
       </c>
@@ -4368,7 +4365,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>198</v>
       </c>
@@ -4460,7 +4457,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>199</v>
       </c>
@@ -4595,9 +4592,8 @@
         <f t="shared" si="0"/>
         <v>2002 RUNSeriesSports</v>
       </c>
-      <c r="N38" s="1" t="e">
-        <f>VLOOKUP(M38,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N38" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -4641,12 +4637,11 @@
         <f t="shared" si="0"/>
         <v>2002 RUNSpecialSports</v>
       </c>
-      <c r="N39" s="1" t="e">
-        <f>VLOOKUP(M39,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>200</v>
       </c>
@@ -4687,9 +4682,8 @@
         <f t="shared" si="0"/>
         <v>2002 RUNSportsSports</v>
       </c>
-      <c r="N40" s="1" t="e">
-        <f>VLOOKUP(M40,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N40" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -4784,7 +4778,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>204</v>
       </c>
@@ -4878,7 +4872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>205</v>
       </c>
@@ -4924,7 +4918,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>205</v>
       </c>
@@ -5016,7 +5010,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>206</v>
       </c>
@@ -5151,9 +5145,8 @@
         <f t="shared" si="0"/>
         <v>2073 RUNSeriesSports</v>
       </c>
-      <c r="N50" s="1" t="e">
-        <f>VLOOKUP(M50,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N50" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -5197,12 +5190,11 @@
         <f t="shared" si="0"/>
         <v>2073 RUNSpecialSports</v>
       </c>
-      <c r="N51" s="1" t="e">
-        <f>VLOOKUP(M51,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N51" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>207</v>
       </c>
@@ -5243,9 +5235,8 @@
         <f t="shared" si="0"/>
         <v>2073 RUNSportsSports</v>
       </c>
-      <c r="N52" s="1" t="e">
-        <f>VLOOKUP(M52,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N52" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -6012,7 +6003,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>218</v>
       </c>
@@ -6104,7 +6095,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>220</v>
       </c>
@@ -6198,7 +6189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>221</v>
       </c>
@@ -6244,7 +6235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>221</v>
       </c>
@@ -6336,7 +6327,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>222</v>
       </c>
@@ -6471,9 +6462,8 @@
         <f t="shared" si="1"/>
         <v>223NovelaSeriesSports</v>
       </c>
-      <c r="N78" s="1" t="e">
-        <f>VLOOKUP(M78,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N78" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -6517,12 +6507,11 @@
         <f t="shared" si="1"/>
         <v>223NovelaSpecialSports</v>
       </c>
-      <c r="N79" s="1" t="e">
-        <f>VLOOKUP(M79,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N79" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>223</v>
       </c>
@@ -6563,9 +6552,8 @@
         <f t="shared" si="1"/>
         <v>223NovelaSportsSports</v>
       </c>
-      <c r="N80" s="1" t="e">
-        <f>VLOOKUP(M80,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N80" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -6614,7 +6602,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>346</v>
       </c>
@@ -6660,7 +6648,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>347</v>
       </c>
@@ -6706,7 +6694,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>348</v>
       </c>
@@ -6893,7 +6881,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>352</v>
       </c>
@@ -6939,7 +6927,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>353</v>
       </c>
@@ -7033,7 +7021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>369</v>
       </c>
@@ -7081,14 +7069,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O91">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Film"/>
-        <filter val="News"/>
-        <filter val="Sports"/>
-        <filter val="Variety"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="13">
       <filters>
         <filter val="#N/A"/>

</xml_diff>

<commit_message>
Changes for scheduling next run in next week
</commit_message>
<xml_diff>
--- a/MasterData/9. AmortTemplateTelemundo.xlsx
+++ b/MasterData/9. AmortTemplateTelemundo.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="61">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -2809,7 +2809,7 @@
   <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,7 +3156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43</v>
       </c>
@@ -3197,9 +3197,8 @@
         <f t="shared" si="0"/>
         <v>432 RUNFilmAcquired Films</v>
       </c>
-      <c r="N8" s="1" t="e">
-        <f>VLOOKUP(M8,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N8" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -7088,7 +7087,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7159,9 +7158,24 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>432 RUNFilmAcquired Films</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>